<commit_message>
Thêm SKU cho sản phẩm
</commit_message>
<xml_diff>
--- a/OnlineStore/wwwroot/templates/ProductImportTemplate.xlsx
+++ b/OnlineStore/wwwroot/templates/ProductImportTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -42,13 +42,16 @@
   </si>
   <si>
     <t>Giá bán</t>
+  </si>
+  <si>
+    <t>SKU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +59,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,13 +90,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -104,8 +135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:G23" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:G23"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Tên sản phẩm"/>
     <tableColumn id="2" name="Mô tả"/>
@@ -381,39 +412,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>